<commit_message>
updated DD per request.
</commit_message>
<xml_diff>
--- a/resources/data-definition/CDS/SubjectSampleMapping_DD.xlsx
+++ b/resources/data-definition/CDS/SubjectSampleMapping_DD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gup2/workspace/vscode/crdcdh/crdc-datahub-backend/resources/data-definition/CDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41DCA69-C94B-2B42-B4AA-C06B8FD3D85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1CD942-900F-5E4A-A849-652F0A369031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="4320" windowWidth="25800" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,16 +45,16 @@
     <t>string</t>
   </si>
   <si>
-    <t>Subject ID</t>
-  </si>
-  <si>
-    <t>Sample ID</t>
-  </si>
-  <si>
     <t>study_participant_id</t>
   </si>
   <si>
     <t>sample_id</t>
+  </si>
+  <si>
+    <t>A sequence of letters, numbers, or characters that uniquely identifies the subject who has taken part in the investigation or research study.</t>
+  </si>
+  <si>
+    <t>A unique sequence of alphanumeric characters used to identify the specimen at it's point of origin.</t>
   </si>
 </sst>
 </file>
@@ -439,15 +439,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="62.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="103.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="2" customWidth="1"/>
@@ -481,10 +478,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -492,10 +489,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>

</xml_diff>